<commit_message>
added to header, trl renaming
</commit_message>
<xml_diff>
--- a/new_data.xlsx
+++ b/new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolf\Downloads\trl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC0A4AC-6DF5-432F-9272-0182AE1B314F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD1333F-609C-4B48-ADE1-B368881CADCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5583" uniqueCount="2389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5587" uniqueCount="2393">
   <si>
     <t>Design of Next Generation Noise And Vibration Sensor Fusion Module</t>
   </si>
@@ -7288,13 +7288,25 @@
   </si>
   <si>
     <t>Prof. Varun Sharma</t>
+  </si>
+  <si>
+    <t>sanjeev.manhas@ece.iitr.ac.in</t>
+  </si>
+  <si>
+    <t>karun.rawat@ece.iitr.ac.in</t>
+  </si>
+  <si>
+    <t>varun.sharma@me.iitr.ac.in</t>
+  </si>
+  <si>
+    <t>varun.sharma@me.iitr. e.in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -7305,6 +7317,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7324,14 +7342,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7634,8 +7655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G932"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C917" workbookViewId="0">
-      <selection activeCell="G940" sqref="G940"/>
+    <sheetView tabSelected="1" topLeftCell="B917" workbookViewId="0">
+      <selection activeCell="D938" sqref="D938"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28986,6 +29007,9 @@
       <c r="C929" s="1" t="s">
         <v>2386</v>
       </c>
+      <c r="D929" s="2" t="s">
+        <v>2389</v>
+      </c>
       <c r="E929" s="1" t="s">
         <v>15</v>
       </c>
@@ -29006,6 +29030,9 @@
       <c r="C930" s="1" t="s">
         <v>2387</v>
       </c>
+      <c r="D930" s="2" t="s">
+        <v>2390</v>
+      </c>
       <c r="E930" s="1" t="s">
         <v>15</v>
       </c>
@@ -29026,6 +29053,9 @@
       <c r="C931" s="1" t="s">
         <v>2388</v>
       </c>
+      <c r="D931" s="2" t="s">
+        <v>2391</v>
+      </c>
       <c r="E931" s="1" t="s">
         <v>237</v>
       </c>
@@ -29046,6 +29076,9 @@
       <c r="C932" s="1" t="s">
         <v>2388</v>
       </c>
+      <c r="D932" s="2" t="s">
+        <v>2392</v>
+      </c>
       <c r="E932" s="1" t="s">
         <v>237</v>
       </c>
@@ -29057,6 +29090,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D929" r:id="rId1" xr:uid="{36DDDC35-1849-45B4-8C35-D88D5DF0D893}"/>
+    <hyperlink ref="D930" r:id="rId2" xr:uid="{8EE1BE26-50B5-4BF4-B82A-2F52E756BC17}"/>
+    <hyperlink ref="D931" r:id="rId3" xr:uid="{8600629C-EB4F-4568-846F-DC0B29B1D062}"/>
+    <hyperlink ref="D932" r:id="rId4" xr:uid="{B1354CD4-BE61-4751-AB68-DB080D28DBA2}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>